<commit_message>
mustafa | replace account & ledger import sameple file & fix universal calender range
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/entries-sample.xlsx
+++ b/src/assets/sample-files/entries-sample.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>EntryDate</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Converted Amount</t>
   </si>
   <si>
     <t>Description</t>
@@ -37,6 +37,9 @@
     <t>TaxRate/TaxUniqueName</t>
   </si>
   <si>
+    <t>Other Tax</t>
+  </si>
+  <si>
     <t>Discount</t>
   </si>
   <si>
@@ -49,31 +52,16 @@
     <t>Unit</t>
   </si>
   <si>
+    <t>27-07-2018</t>
+  </si>
+  <si>
+    <t>cash</t>
+  </si>
+  <si>
     <t>sales</t>
   </si>
   <si>
-    <t>cash</t>
-  </si>
-  <si>
-    <t>credit</t>
-  </si>
-  <si>
-    <t>discount check</t>
-  </si>
-  <si>
-    <t>gst18</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>nos</t>
-  </si>
-  <si>
-    <t>debit</t>
-  </si>
-  <si>
-    <t>without tax</t>
+    <t>test accounts</t>
   </si>
 </sst>
 </file>
@@ -81,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm-dd-yyyy"/>
+    <numFmt numFmtId="164" formatCode="d&quot;/&quot;m&quot;/&quot;yy"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -90,11 +78,12 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,7 +93,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border/>
     <border>
       <left style="thin">
@@ -116,6 +105,36 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -124,17 +143,38 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -163,105 +203,71 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
-        <v>43348.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="D2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="6">
+        <v>500.0</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1000.0</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>43348.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
all assets file changed
</commit_message>
<xml_diff>
--- a/src/assets/sample-files/entries-sample.xlsx
+++ b/src/assets/sample-files/entries-sample.xlsx
@@ -61,7 +61,7 @@
     <t>Invoice Number</t>
   </si>
   <si>
-    <t>01/31/2019</t>
+    <t>09/01/2019</t>
   </si>
   <si>
     <t>Cash</t>
@@ -221,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -235,7 +235,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -245,6 +245,9 @@
     </xf>
     <xf borderId="4" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -366,7 +369,7 @@
       <c r="P2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -382,22 +385,22 @@
       <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="K3" s="7"/>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>27</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="9" t="s">
         <v>29</v>
       </c>
       <c r="O3" s="7" t="s">
@@ -408,7 +411,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -426,7 +429,7 @@
         <v>34</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="10" t="s">
         <v>35</v>
       </c>
       <c r="J4" s="7"/>

</xml_diff>